<commit_message>
fixed errors in excel
</commit_message>
<xml_diff>
--- a/Code/All dataset.xlsx
+++ b/Code/All dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssa/code/alyssageorgee/group23/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA80D0F-2FB2-724E-B6A8-3E06C54151DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E639437E-9DB8-B143-B597-1E115ACFB7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="15800" xr2:uid="{EF997A0B-C278-2140-872F-D8857E89B0A9}"/>
   </bookViews>
@@ -111,21 +111,12 @@
     <t>Redbridge</t>
   </si>
   <si>
-    <t>Richmond upon Thanes</t>
-  </si>
-  <si>
     <t>Wandsworth</t>
   </si>
   <si>
     <t>Hammersmith and Fulham</t>
   </si>
   <si>
-    <t xml:space="preserve">Kensington and Chelsea </t>
-  </si>
-  <si>
-    <t>Westminser</t>
-  </si>
-  <si>
     <t>Camden</t>
   </si>
   <si>
@@ -154,6 +145,15 @@
   </si>
   <si>
     <t>Suicide Rates (2019) (in %)</t>
+  </si>
+  <si>
+    <t>Richmond upon Thames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kensington and Chelsea	</t>
+  </si>
+  <si>
+    <t>Westminster</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE956E78-015E-C346-AA3F-695F205998D1}">
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,22 +617,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
     </row>
     <row r="21" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1">
         <v>7.0999999999999994E-2</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="23" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
         <v>7.8E-2</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="24" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>6.6000000000000003E-2</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="25" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1">
         <v>8.3000000000000004E-2</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="26" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <v>2.88</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="27" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>9.1999999999999998E-2</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="29" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>0.104</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="30" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>0.106</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="32" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>6.0999999999999999E-2</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="33" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B33" s="6">
         <v>8.1000000000000003E-2</v>

</xml_diff>